<commit_message>
UPDATED TILL - 01-09-2020
</commit_message>
<xml_diff>
--- a/system-client/API/import_bulk_order.xlsx
+++ b/system-client/API/import_bulk_order.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\My PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33A5841-B8C5-46F3-8552-9BA015CB0B1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11385" windowHeight="2490"/>
   </bookViews>
   <sheets>
     <sheet name="Criminal Court- Sample Template" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="329">
   <si>
     <t>Request ID</t>
   </si>
@@ -43,34 +42,976 @@
     <t>Country</t>
   </si>
   <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Aland Islands</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Anguilla</t>
+  </si>
+  <si>
+    <t>Antarctica</t>
+  </si>
+  <si>
+    <t>Antigua And Barbuda</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bahamas The</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Bouvet Island</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>British Indian Ocean Territory</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Christmas Island</t>
+  </si>
+  <si>
+    <t>Cocos (Keeling) Islands</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Congo The Democratic Republic Of The</t>
+  </si>
+  <si>
+    <t>Cook Islands</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Cote D'Ivoire (Ivory Coast)</t>
+  </si>
+  <si>
+    <t>Croatia (Hrvatska)</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>East Timor</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Falkland Islands</t>
+  </si>
+  <si>
+    <t>Faroe Islands</t>
+  </si>
+  <si>
+    <t>Fiji Islands</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>French Guiana</t>
+  </si>
+  <si>
+    <t>French Polynesia</t>
+  </si>
+  <si>
+    <t>French Southern Territories</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Gambia The</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Gibraltar</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Guadeloupe</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guernsey and Alderney</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Heard and McDonald Islands</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Hong Kong S.A.R.</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
     <t>India</t>
   </si>
   <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>Korea North</t>
+  </si>
+  <si>
+    <t>Korea South</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Macau S.A.R.</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Man (Isle of)</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Martinique</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Mayotte</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Montserrat</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Netherlands Antilles</t>
+  </si>
+  <si>
+    <t>Netherlands The</t>
+  </si>
+  <si>
+    <t>New Caledonia</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Niue</t>
+  </si>
+  <si>
+    <t>Norfolk Island</t>
+  </si>
+  <si>
+    <t>Northern Mariana Islands</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>Palestinian Territory Occupied</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Papua new Guinea</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Pitcairn Island</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Reunion</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Saint Helena</t>
+  </si>
+  <si>
+    <t>Saint Kitts And Nevis</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Saint Pierre and Miquelon</t>
+  </si>
+  <si>
+    <t>Saint Vincent And The Grenadines</t>
+  </si>
+  <si>
+    <t>Saint-Barthelemy</t>
+  </si>
+  <si>
+    <t>Saint-Martin (French part)</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>South Georgia</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>Svalbard And Jan Mayen Islands</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Tokelau</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Trinidad And Tobago</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Turks And Caicos Islands</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>United States Minor Outlying Islands</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Vatican City State (Holy See)</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Virgin Islands (British)</t>
+  </si>
+  <si>
+    <t>Virgin Islands (US)</t>
+  </si>
+  <si>
+    <t>Wallis And Futuna Islands</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
     <t>Applicant Name</t>
   </si>
   <si>
-    <t>Swapnali Thorat</t>
-  </si>
-  <si>
-    <t>Pune Mumbai Road</t>
-  </si>
-  <si>
-    <t>TESTING</t>
-  </si>
-  <si>
-    <t>Prasad.Jadhav</t>
-  </si>
-  <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
-    <t>Pramod</t>
+    <t>AB00001</t>
+  </si>
+  <si>
+    <t>Rohan Das</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Check his identity</t>
+  </si>
+  <si>
+    <t>AB00002</t>
+  </si>
+  <si>
+    <t>2020-24-08-7752dc-1</t>
+  </si>
+  <si>
+    <t>TL-081920-9A485-PL-004</t>
+  </si>
+  <si>
+    <t>GA-081920-329C9-CJ-004</t>
+  </si>
+  <si>
+    <t>GA-082120-334BV-CJ-002</t>
+  </si>
+  <si>
+    <t>GA-082520-336W4-CJ-001</t>
+  </si>
+  <si>
+    <t>GA-082520-3372M-CJ-002</t>
+  </si>
+  <si>
+    <t>GA-082520-3372X-CJ-001</t>
+  </si>
+  <si>
+    <t>GA-082520-3372Z-CJ-001</t>
+  </si>
+  <si>
+    <t>GC-082520-336FQ-CJ-001</t>
+  </si>
+  <si>
+    <t>GA-082520-3378M-CJ-001</t>
+  </si>
+  <si>
+    <t>GT-082520-337A2-CJ-001</t>
+  </si>
+  <si>
+    <t>GC-082520-336G7-CJ-001</t>
+  </si>
+  <si>
+    <t>GA-082620-337PR-CJ-001</t>
+  </si>
+  <si>
+    <t>Suresh Singh Kaushalya</t>
+  </si>
+  <si>
+    <t>Natarajan Venkataraman</t>
+  </si>
+  <si>
+    <t>Sahana Muthu Muthu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heena . Rathi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madhur Makkar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandeep Singh Singh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nimish Kapoor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaushal Kumar, Singh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dineshkumar Ramasamy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shreya Dineshbhai ,Thummar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheetal Vernekar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swathi K S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sangeetha Govindaraj </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandesha P, S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devendrakumar Bherulal, Rajawat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rukhsana Syed </t>
+  </si>
+  <si>
+    <t>â€œKamalalayamâ€, Plot No 29, New  No 7,  Kumaran Nagar 3rd Cross Street,  Virugambakkam</t>
+  </si>
+  <si>
+    <t>E202, Ceebros Belvedere, Classic Farms Avenue, Sholinganallur</t>
+  </si>
+  <si>
+    <t>D/14, 208, HIG Flats, Golden Jubliee Apartments, Anna Main Road, KK Nagar</t>
+  </si>
+  <si>
+    <t>Great Lakes Institute of Management, Dr. Bala V. Balachandar Campus, East Coast Road,Manamai Village Thirukazhukundram, Taluk, Manamai</t>
+  </si>
+  <si>
+    <t>21/788, C, Golden Castle Apartment, Ramasamy Salai, KK Nagar</t>
+  </si>
+  <si>
+    <t>Zolo Yin, No.94, Sudarshan Tower 2nd Cross, Krishna Reddy Layou Konnappan Agrahara, Electronic City Phase 2</t>
+  </si>
+  <si>
+    <t>Pan Oasis, Sector 70, Noida, Uttar Pradesh, 201301, India</t>
+  </si>
+  <si>
+    <t>B4-15 3rd Floor Sector 17 Rohini New Delhi, 110085</t>
+  </si>
+  <si>
+    <t>01, Shanta mhal , Golf course , Bangalore , Karnataka , 560052</t>
+  </si>
+  <si>
+    <t>84, Ward No 11, Mohalla Panditan, Degree College Poonch, Poonch, 185101, Jammu and Kashmir, India</t>
+  </si>
+  <si>
+    <t>Gyan lok colony , Near Shivam Lodge , Bulandshahr , Uttar Pradesh , 203131</t>
+  </si>
+  <si>
+    <t>101, #8/3/2, Akshaya Residency, 1st Cross, 1st A Main, Sri Byreshwara Layout, Hennur Bande, Near Has, Bangalore, 560043, KARNATAKA, India</t>
+  </si>
+  <si>
+    <t>502 , Building A , Rajhans Elita , Pal RTO, Surat , Gujarat , 395009</t>
+  </si>
+  <si>
+    <t>C/O Ravindra Naik,M.H Naik compound, Kalamma nagar, Yellapur, 581359, Karnataka, India</t>
+  </si>
+  <si>
+    <t>565, 13th cross, Bright Way School Road, Gowdanapalya, Uttarahalli Main Road, Subramanyapura Post, S, Bangalore, 560061, Karnataka, India</t>
+  </si>
+  <si>
+    <t>No.32, Door No 1/903 First floor Rukmani Nagar, Medavakkam, Chennai, 600100, Tamil Nadu, India</t>
+  </si>
+  <si>
+    <t>#54/2 Puttanahalli Village, Soraba Taluk, Shivamogga, 577419, Karnataka, India</t>
+  </si>
+  <si>
+    <t>31, 28, Ekta Society, M.G Road, Vishnunagar, Opposite Railway Station, Dombivli(West), Mumbai, 421202, MAHARASHTRA, India</t>
+  </si>
+  <si>
+    <t>15-1-174/2, Nehru Nagar, Macherla, Guntur, 522426, Andhra Pradesh, India</t>
+  </si>
+  <si>
+    <t>VENKATARAMAN RAMASAMY</t>
+  </si>
+  <si>
+    <t>Muthu Rajapandian Malaivelu Muthusamy</t>
+  </si>
+  <si>
+    <t>Gopal Shankar Rathi</t>
+  </si>
+  <si>
+    <t>Krishan Kumar Makkar</t>
+  </si>
+  <si>
+    <t>Balli Village</t>
+  </si>
+  <si>
+    <t>Rahul Kapoor</t>
+  </si>
+  <si>
+    <t>Devendra singh</t>
+  </si>
+  <si>
+    <t>Ramasamy E</t>
+  </si>
+  <si>
+    <t>Dinesh Thummar</t>
+  </si>
+  <si>
+    <t>Shivanand B Vernekar</t>
+  </si>
+  <si>
+    <t>Sampath Kumar K R</t>
+  </si>
+  <si>
+    <t>Govindaraj N</t>
+  </si>
+  <si>
+    <t>Shivappa P S</t>
+  </si>
+  <si>
+    <t>Bherulal Rajawat</t>
+  </si>
+  <si>
+    <t>Syed Mahaboob Jani</t>
+  </si>
+  <si>
+    <t>Kindly use this address details for verification  : Pan Oasis, Sector 70, Noida, Uttar Pradesh, 201301, India,district: Gautam Buddha Nagar"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kindly share amended report with Address line - B4-15 3rd Floor Sector 17 Rohini New Delhi, 110085 , Delhi , North Delhi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kindly use this details for verification  : father's name "Kalyan singh" </t>
+  </si>
+  <si>
+    <t>a-16, Reet street</t>
+  </si>
+  <si>
+    <t>Yamin bazar,</t>
+  </si>
+  <si>
+    <t>roa saheb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
@@ -585,7 +1526,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -601,6 +1542,19 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -737,23 +1691,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -789,23 +1726,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -981,11 +1901,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFB247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1000,12 +1920,12 @@
     <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>8</v>
+        <v>254</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1025,83 +1945,1696 @@
       <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1234</v>
+      <c r="XFB1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="9">
+        <v>30985</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="9">
+        <v>27851</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
-        <v>34593</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="9">
+        <v>33606</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="1" t="s">
+    </row>
+    <row r="5" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>40105611</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="9">
+        <v>33606</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1501</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="6" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>51694712</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="9">
+        <v>33606</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="7" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>51694712</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C7" s="9">
+        <v>33606</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="8" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>51694712</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C8" s="9">
+        <v>33606</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1234</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2">
-        <v>34593</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1501</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>7</v>
+    <row r="9" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>51694712</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="9">
+        <v>33759</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>51694712</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" s="9">
+        <v>34501</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" s="9">
+        <v>35221</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C12" s="9">
+        <v>35535</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB12" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" s="9">
+        <v>35065</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB13" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C14" s="9">
+        <v>33412</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB14" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C15" s="9">
+        <v>36260</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" s="9">
+        <v>35903</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB16" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" s="9">
+        <v>32957</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB17" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C18" s="9">
+        <v>31942</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="9">
+        <v>33340</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB19" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C20" s="9">
+        <v>34100</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB20" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C21" s="9">
+        <v>34748</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C22" s="10">
+        <v>32586</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="XFB22" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="XFB23" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB24" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB25" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB26" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB27" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB28" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB29" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB30" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB31" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB32" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB33" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB34" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB35" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB36" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB37" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB38" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB39" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB40" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB41" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB42" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB43" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB44" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB45" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB46" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB47" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB48" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB49" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB50" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB51" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB52" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB53" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB54" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB55" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB56" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB57" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB58" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB59" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB60" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB61" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB62" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB63" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB64" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB65" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB66" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB67" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB68" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB69" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB70" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB71" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB72" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB73" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB74" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB75" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB76" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB77" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB78" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB79" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB80" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB81" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB82" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB83" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB84" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB85" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="86" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB86" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB87" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB88" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="89" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB89" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB90" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="91" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB91" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="92" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB92" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="93" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB93" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB94" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB95" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="96" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB96" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB97" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB98" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="99" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB99" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="100" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB100" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="101" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB101" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="102" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB102" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="103" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB103" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="104" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB104" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="105" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB105" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="106" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB106" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="107" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB107" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="108" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB108" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="109" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB109" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="110" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB110" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="111" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB111" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="112" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB112" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="113" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB113" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="114" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB114" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="115" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB115" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="116" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB116" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="117" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB117" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="118" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB118" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="119" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB119" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB120" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="121" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB121" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="122" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB122" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="123" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB123" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="124" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB124" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="125" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB125" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="126" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB126" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="127" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB127" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="128" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB128" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="129" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB129" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="130" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB130" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="131" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB131" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="132" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB132" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="133" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB133" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="134" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB134" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="135" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB135" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="136" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB136" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="137" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB137" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="138" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB138" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="139" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB139" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="140" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB140" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="141" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB141" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="142" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB142" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="143" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB143" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="144" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB144" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="145" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB145" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="146" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB146" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="147" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB147" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="148" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB148" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="149" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB149" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="150" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB150" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="151" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB151" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="152" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB152" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="153" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB153" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="154" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB154" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="155" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB155" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="156" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB156" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="157" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB157" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="158" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB158" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="159" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB159" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="160" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB160" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="161" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB161" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="162" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB162" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="163" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB163" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="164" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB164" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="165" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB165" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="166" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB166" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="167" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB167" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="168" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB168" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="169" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB169" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="170" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB170" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="171" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB171" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="172" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB172" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="173" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB173" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="174" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB174" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="175" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB175" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="176" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB176" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="177" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB177" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="178" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB178" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="179" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB179" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="180" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB180" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="181" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB181" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="182" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB182" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="183" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB183" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="184" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB184" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="185" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB185" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="186" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB186" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="187" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB187" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="188" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB188" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="189" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB189" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="190" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB190" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="191" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB191" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="192" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB192" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="193" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB193" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="194" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB194" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="195" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB195" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="196" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB196" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="197" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB197" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="198" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB198" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="199" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB199" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="200" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB200" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="201" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB201" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="202" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB202" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="203" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB203" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="204" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB204" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="205" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB205" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="206" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB206" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="207" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB207" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="208" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB208" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="209" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB209" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="210" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB210" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="211" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB211" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="212" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB212" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="213" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB213" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="214" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB214" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="215" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB215" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="216" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB216" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="217" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB217" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="218" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB218" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="219" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB219" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="220" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB220" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="221" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB221" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="222" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB222" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="223" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB223" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="224" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB224" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="225" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB225" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="226" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB226" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="227" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB227" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="228" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB228" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="229" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB229" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="230" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB230" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="231" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB231" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="232" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB232" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="233" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB233" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="234" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB234" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="235" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB235" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="236" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB236" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="237" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB237" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="238" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB238" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="239" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB239" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="240" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB240" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="241" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB241" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="242" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB242" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="243" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB243" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="244" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB244" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="245" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB245" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="246" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB246" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="247" spans="16382:16382" x14ac:dyDescent="0.25">
+      <c r="XFB247" s="5" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="rrYQXS0guFSrp+7cIxSUx3wMfY70pfUpaMYGkOPk6iqa+KhOLo3CuD4cXOhShq9T71fDnwQ6zrXGqJmhsC+vwA==" saltValue="i6HOqabSScmvl9lqydy6HQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{BE3E2F5A-540D-4361-9FE3-8903C1072227}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
       <formula1>$XFB$1:$XFB$247</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
COMMIT - UPDATED TILL - 29-09-2020
COMMIT - UPDATED TILL - 29-09-2020
</commit_message>
<xml_diff>
--- a/system-client/API/import_bulk_order.xlsx
+++ b/system-client/API/import_bulk_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3014A4-52A0-44AD-A494-EC20A5E85C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CBD88A-39C4-4090-876D-AFD3C2FA1349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Request ID</t>
   </si>
@@ -61,6 +61,30 @@
   </si>
   <si>
     <t>INDIA</t>
+  </si>
+  <si>
+    <t>IR003</t>
+  </si>
+  <si>
+    <t>Sujata</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>MUMBAI</t>
+  </si>
+  <si>
+    <t>DELHI</t>
   </si>
 </sst>
 </file>
@@ -988,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1053,6 +1077,45 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
UPDATED TILL - 14-10-2020
UPDATED TILL - 14-10-2020
</commit_message>
<xml_diff>
--- a/system-client/API/import_bulk_order.xlsx
+++ b/system-client/API/import_bulk_order.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Puneet\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CBD88A-39C4-4090-876D-AFD3C2FA1349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9075"/>
   </bookViews>
   <sheets>
     <sheet name="Criminal Court- Sample Template" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Request ID</t>
   </si>
@@ -48,49 +47,82 @@
 FIRST_NAME.LAST_NAME</t>
   </si>
   <si>
-    <t>IR002</t>
-  </si>
-  <si>
-    <t>SUJATA.THORAT</t>
-  </si>
-  <si>
-    <t>PUNE</t>
-  </si>
-  <si>
-    <t>MOHAN</t>
-  </si>
-  <si>
-    <t>INDIA</t>
-  </si>
-  <si>
-    <t>IR003</t>
-  </si>
-  <si>
-    <t>Sujata</t>
-  </si>
-  <si>
-    <t>IND</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>MUMBAI</t>
-  </si>
-  <si>
-    <t>DELHI</t>
+    <t>HA-100520-HW2G5-PL-001</t>
+  </si>
+  <si>
+    <t>GO-100520-HW3BT-PL-001</t>
+  </si>
+  <si>
+    <t>HA-100520-HY4KJ-PL-008</t>
+  </si>
+  <si>
+    <t>TL-100520-J23C3-PL-001</t>
+  </si>
+  <si>
+    <t>HA-100520-HZ3ZJ-PL-004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamanna . Vidhwani </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girish . Naik </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayank Pratap. Tyagi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meher Deepthi . Rokkam </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEJAS RAMESH, SHINGE </t>
+  </si>
+  <si>
+    <t>09, Vidyut Nagar, Sindhi Colony- Gali No. 2, Patel Bhawan, Khandwa, 450001, Madhya Pradesh, India</t>
+  </si>
+  <si>
+    <t>India, Maharashtra, Mumbai, 400092, 201, Khyati Deep CHS, Satya Sai Complex, Padma Nagar Road, Chikuwadi, Borivali (W)</t>
+  </si>
+  <si>
+    <t>39/4, PWD COLONY, Jodhpur, 342001, India</t>
+  </si>
+  <si>
+    <t>17,5A,SAHYADRI CO.HSG.SCO.,MUMBAI-PUNA ROAD, KALWA (W),THANE, Maharashtra, India-400605</t>
+  </si>
+  <si>
+    <t>D-306, Shree Vardhman Mantra, Sector 67, Gurugram, 122102, Haryana, India</t>
+  </si>
+  <si>
+    <t>Smt.Lalitha Shashtri Hostel,Rose Residency Complex,Sector-19,DWARKA, Delhi, India-110075</t>
+  </si>
+  <si>
+    <t>Jayram Kundandas Vidhwani</t>
+  </si>
+  <si>
+    <t>RAMESH TAYAPPA SHINGE</t>
+  </si>
+  <si>
+    <t>Dinesh Kumar Mathur</t>
+  </si>
+  <si>
+    <t>VASUDEV SITARAM NAIK</t>
+  </si>
+  <si>
+    <t>Sudarsana Rao Rokkam</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>19-15-1988</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
@@ -767,23 +799,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -819,23 +834,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1011,19 +1009,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="21" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21" style="2" customWidth="1"/>
+    <col min="4" max="4" width="119.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="17.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="5"/>
@@ -1061,59 +1059,125 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3">
-        <v>35509</v>
+        <v>35597</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="H2" s="5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>31924</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="3">
+        <v>33723</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>34050</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATED TILL - 22-10-2020
UPDATED TILL - 22-10-2020
</commit_message>
<xml_diff>
--- a/system-client/API/import_bulk_order.xlsx
+++ b/system-client/API/import_bulk_order.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9075"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Criminal Court- Sample Template" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Request ID</t>
   </si>
@@ -47,67 +47,28 @@
 FIRST_NAME.LAST_NAME</t>
   </si>
   <si>
-    <t>HA-100520-HW2G5-PL-001</t>
-  </si>
-  <si>
-    <t>GO-100520-HW3BT-PL-001</t>
-  </si>
-  <si>
-    <t>HA-100520-HY4KJ-PL-008</t>
-  </si>
-  <si>
-    <t>TL-100520-J23C3-PL-001</t>
-  </si>
-  <si>
-    <t>HA-100520-HZ3ZJ-PL-004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tamanna . Vidhwani </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Girish . Naik </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mayank Pratap. Tyagi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meher Deepthi . Rokkam </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEJAS RAMESH, SHINGE </t>
-  </si>
-  <si>
-    <t>09, Vidyut Nagar, Sindhi Colony- Gali No. 2, Patel Bhawan, Khandwa, 450001, Madhya Pradesh, India</t>
-  </si>
-  <si>
-    <t>India, Maharashtra, Mumbai, 400092, 201, Khyati Deep CHS, Satya Sai Complex, Padma Nagar Road, Chikuwadi, Borivali (W)</t>
-  </si>
-  <si>
-    <t>39/4, PWD COLONY, Jodhpur, 342001, India</t>
-  </si>
-  <si>
-    <t>17,5A,SAHYADRI CO.HSG.SCO.,MUMBAI-PUNA ROAD, KALWA (W),THANE, Maharashtra, India-400605</t>
-  </si>
-  <si>
-    <t>D-306, Shree Vardhman Mantra, Sector 67, Gurugram, 122102, Haryana, India</t>
-  </si>
-  <si>
-    <t>Smt.Lalitha Shashtri Hostel,Rose Residency Complex,Sector-19,DWARKA, Delhi, India-110075</t>
-  </si>
-  <si>
-    <t>Jayram Kundandas Vidhwani</t>
-  </si>
-  <si>
-    <t>RAMESH TAYAPPA SHINGE</t>
-  </si>
-  <si>
-    <t>Dinesh Kumar Mathur</t>
-  </si>
-  <si>
-    <t>VASUDEV SITARAM NAIK</t>
-  </si>
-  <si>
-    <t>Sudarsana Rao Rokkam</t>
+    <t xml:space="preserve">Dinesh Kannan  Muthiah </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kishore  Yama </t>
+  </si>
+  <si>
+    <t>Plot No 32 Aavin Nagar  , Anna Nagar , Gandhi Nagar , Alavandan ,  Madurai ,  625020 ,  Tamil Nadu ,  India</t>
+  </si>
+  <si>
+    <t>G2 ,  SAI TEJA RESIDENCY ,  ROAD NO.1 BHANDARI LAYOUT ,  NIZAMPET ,  NEAR SAMSKRUTI SCHOOL ,  HYDERABAD ,  500090 ,  Telangana ,  India</t>
+  </si>
+  <si>
+    <t>House no. 217 near Hanuman temple  , village gwali  , teh jawar  , Dist : Sehore , Madhya Pradesh ,  India - 466118</t>
+  </si>
+  <si>
+    <t>Muthiah</t>
+  </si>
+  <si>
+    <t>MOHAN RAO YAMA</t>
+  </si>
+  <si>
+    <t>Munnalal Patidar</t>
   </si>
   <si>
     <t>General</t>
@@ -116,7 +77,16 @@
     <t>India</t>
   </si>
   <si>
-    <t>19-15-1988</t>
+    <t>HEGT-1020-069svsf</t>
+  </si>
+  <si>
+    <t>HEGT-1020-06slvsv</t>
+  </si>
+  <si>
+    <t>HEGT-1020-0lsndvksv</t>
+  </si>
+  <si>
+    <t>19-15-1900</t>
   </si>
 </sst>
 </file>
@@ -284,7 +254,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,6 +437,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,7 +622,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
@@ -665,6 +641,8 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1010,19 +988,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="3" customWidth="1"/>
-    <col min="4" max="4" width="119.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="123.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="5"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
@@ -1055,130 +1034,223 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3">
-        <v>35597</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="9">
+        <v>29266</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B4"/>
+      <c r="C4" s="9">
+        <v>34315</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3">
-        <v>31924</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3">
-        <v>33723</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="A5" s="8"/>
+      <c r="B5"/>
+      <c r="C5" s="9"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3">
-        <v>34050</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="A6" s="8"/>
+      <c r="B6"/>
+      <c r="C6" s="9"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="A7" s="8"/>
+      <c r="B7"/>
+      <c r="C7" s="9"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8"/>
+      <c r="C8" s="9"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9"/>
+      <c r="C9" s="9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10"/>
+      <c r="C10" s="9"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11"/>
+      <c r="C11" s="9"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12"/>
+      <c r="C12" s="9"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13"/>
+      <c r="C13" s="9"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14"/>
+      <c r="C14" s="9"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15"/>
+      <c r="C15" s="9"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16"/>
+      <c r="C16" s="9"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17"/>
+      <c r="C17" s="9"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18"/>
+      <c r="C18" s="9"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19"/>
+      <c r="C19" s="9"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20"/>
+      <c r="C20" s="9"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21"/>
+      <c r="C21" s="9"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22"/>
+      <c r="C22" s="9"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23"/>
+      <c r="C23" s="9"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>